<commit_message>
trial balance is done...
</commit_message>
<xml_diff>
--- a/public/report.xlsx
+++ b/public/report.xlsx
@@ -73,9 +73,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -101,9 +110,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -404,35 +419,44 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A5" sqref="A5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="21.137695" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="31.706543" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -452,7 +476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -472,7 +496,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -492,20 +516,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="A5:E5"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>